<commit_message>
african flags and  maps
</commit_message>
<xml_diff>
--- a/sub_pro_0_tutorials_tools/single_countries/datasets/africa_countries_capitals.xlsx
+++ b/sub_pro_0_tutorials_tools/single_countries/datasets/africa_countries_capitals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_Files\afro_dataviz\sub_pro_0_tutorials_tools\single_countries\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{360E9273-C64F-40DB-A532-1815735DD003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76198959-13EF-45DE-BB3F-AAC2FF9575E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A1E12BD6-AB20-402E-A601-F1B44C45C93F}"/>
+    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{A1E12BD6-AB20-402E-A601-F1B44C45C93F}"/>
   </bookViews>
   <sheets>
     <sheet name="africa_countries_capitals" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
   <si>
     <t>Country</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Asmara</t>
   </si>
   <si>
-    <t>Eswatini</t>
-  </si>
-  <si>
     <t>Mbabane</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
     <t>Kigali</t>
   </si>
   <si>
-    <t>São Tomé and Príncipe</t>
-  </si>
-  <si>
     <t>São Tomé</t>
   </si>
   <si>
@@ -353,6 +347,15 @@
   </si>
   <si>
     <t>Harare</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>eSwatini</t>
+  </si>
+  <si>
+    <t>São Tomé and Principe</t>
   </si>
 </sst>
 </file>
@@ -1193,9 +1196,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14589FB-9308-4EBF-A6B3-B0546CA38C1B}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1203,7 +1208,7 @@
     <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1217,7 +1222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1225,13 +1230,16 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>36.753799999999998</v>
+        <v>36.8740107224518</v>
       </c>
       <c r="D2">
-        <v>3.0588000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3.4881161987262002</v>
+      </c>
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1239,13 +1247,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>-8.8383000000000003</v>
+        <v>-8.6382065872055698</v>
       </c>
       <c r="D3">
-        <v>13.234400000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>14.0434411543779</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1259,7 +1267,7 @@
         <v>2.6288999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1273,7 +1281,7 @@
         <v>25.923100000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1287,7 +1295,7 @@
         <v>-1.5197000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1301,7 +1309,7 @@
         <v>29.930599999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1315,7 +1323,7 @@
         <v>-23.513300000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1329,7 +1337,7 @@
         <v>11.5021</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1343,7 +1351,7 @@
         <v>18.558199999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1357,7 +1365,7 @@
         <v>15.0557</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1371,7 +1379,7 @@
         <v>43.255099999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1385,7 +1393,7 @@
         <v>15.266299999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1399,7 +1407,7 @@
         <v>15.242900000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1413,7 +1421,7 @@
         <v>-5.2892999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1471,10 +1479,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
         <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
       </c>
       <c r="C20">
         <v>-26.305399999999999</v>
@@ -1485,10 +1493,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
         <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
       </c>
       <c r="C21">
         <v>9.0299999999999994</v>
@@ -1499,10 +1507,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
       </c>
       <c r="C22">
         <v>0.41620000000000001</v>
@@ -1513,10 +1521,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
         <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>46</v>
       </c>
       <c r="C23">
         <v>13.4549</v>
@@ -1527,10 +1535,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
         <v>47</v>
-      </c>
-      <c r="B24" t="s">
-        <v>48</v>
       </c>
       <c r="C24">
         <v>5.6036999999999999</v>
@@ -1541,10 +1549,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
         <v>49</v>
-      </c>
-      <c r="B25" t="s">
-        <v>50</v>
       </c>
       <c r="C25">
         <v>9.6411999999999995</v>
@@ -1555,10 +1563,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
         <v>51</v>
-      </c>
-      <c r="B26" t="s">
-        <v>52</v>
       </c>
       <c r="C26">
         <v>11.8636</v>
@@ -1569,10 +1577,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
         <v>53</v>
-      </c>
-      <c r="B27" t="s">
-        <v>54</v>
       </c>
       <c r="C27">
         <v>-1.2864</v>
@@ -1583,10 +1591,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
         <v>55</v>
-      </c>
-      <c r="B28" t="s">
-        <v>56</v>
       </c>
       <c r="C28">
         <v>-29.315799999999999</v>
@@ -1597,10 +1605,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
         <v>57</v>
-      </c>
-      <c r="B29" t="s">
-        <v>58</v>
       </c>
       <c r="C29">
         <v>6.3155999999999999</v>
@@ -1611,10 +1619,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
         <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
       </c>
       <c r="C30">
         <v>32.8872</v>
@@ -1625,10 +1633,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
         <v>61</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
       </c>
       <c r="C31">
         <v>-18.879200000000001</v>
@@ -1639,10 +1647,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
         <v>63</v>
-      </c>
-      <c r="B32" t="s">
-        <v>64</v>
       </c>
       <c r="C32">
         <v>-13.9833</v>
@@ -1653,10 +1661,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
         <v>65</v>
-      </c>
-      <c r="B33" t="s">
-        <v>66</v>
       </c>
       <c r="C33">
         <v>12.639200000000001</v>
@@ -1667,10 +1675,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
         <v>67</v>
-      </c>
-      <c r="B34" t="s">
-        <v>68</v>
       </c>
       <c r="C34">
         <v>18.077999999999999</v>
@@ -1681,10 +1689,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
         <v>69</v>
-      </c>
-      <c r="B35" t="s">
-        <v>70</v>
       </c>
       <c r="C35">
         <v>-20.160900000000002</v>
@@ -1695,10 +1703,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
         <v>71</v>
-      </c>
-      <c r="B36" t="s">
-        <v>72</v>
       </c>
       <c r="C36">
         <v>34.020899999999997</v>
@@ -1709,10 +1717,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
         <v>73</v>
-      </c>
-      <c r="B37" t="s">
-        <v>74</v>
       </c>
       <c r="C37">
         <v>-25.969200000000001</v>
@@ -1723,10 +1731,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
         <v>75</v>
-      </c>
-      <c r="B38" t="s">
-        <v>76</v>
       </c>
       <c r="C38">
         <v>-22.559699999999999</v>
@@ -1737,10 +1745,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
         <v>77</v>
-      </c>
-      <c r="B39" t="s">
-        <v>78</v>
       </c>
       <c r="C39">
         <v>13.5128</v>
@@ -1751,10 +1759,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
         <v>79</v>
-      </c>
-      <c r="B40" t="s">
-        <v>80</v>
       </c>
       <c r="C40">
         <v>9.0579000000000001</v>
@@ -1765,10 +1773,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
         <v>81</v>
-      </c>
-      <c r="B41" t="s">
-        <v>82</v>
       </c>
       <c r="C41">
         <v>-1.9440999999999999</v>
@@ -1779,10 +1787,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C42">
         <v>0.33650000000000002</v>
@@ -1793,10 +1801,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C43">
         <v>14.6928</v>
@@ -1807,10 +1815,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C44">
         <v>-4.6191000000000004</v>
@@ -1821,10 +1829,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C45">
         <v>8.4657</v>
@@ -1835,10 +1843,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C46">
         <v>2.0468999999999999</v>
@@ -1849,10 +1857,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C47">
         <v>-25.747900000000001</v>
@@ -1863,10 +1871,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C48">
         <v>4.8593999999999999</v>
@@ -1877,10 +1885,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C49">
         <v>15.5007</v>
@@ -1891,10 +1899,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C50">
         <v>-6.1630000000000003</v>
@@ -1905,10 +1913,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51">
         <v>6.1725000000000003</v>
@@ -1919,10 +1927,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B52" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C52">
         <v>36.8065</v>
@@ -1933,10 +1941,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C53">
         <v>0.34760000000000002</v>
@@ -1947,10 +1955,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54">
         <v>-15.387499999999999</v>
@@ -1961,10 +1969,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C55">
         <v>-17.8292</v>

</xml_diff>

<commit_message>
new regional grouping images
</commit_message>
<xml_diff>
--- a/sub_pro_0_tutorials_tools/single_countries/datasets/africa_countries_capitals.xlsx
+++ b/sub_pro_0_tutorials_tools/single_countries/datasets/africa_countries_capitals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_Files\afro_dataviz\sub_pro_0_tutorials_tools\single_countries\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76198959-13EF-45DE-BB3F-AAC2FF9575E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97CF004-1635-40D1-B88E-1599D821AA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{A1E12BD6-AB20-402E-A601-F1B44C45C93F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A1E12BD6-AB20-402E-A601-F1B44C45C93F}"/>
   </bookViews>
   <sheets>
     <sheet name="africa_countries_capitals" sheetId="1" r:id="rId1"/>
@@ -839,8 +839,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1198,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14589FB-9308-4EBF-A6B3-B0546CA38C1B}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1209,16 +1210,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>